<commit_message>
modified:   data/2024Q2_29012025.xlsx modified:   data/2024Q3map.xlsx modified:   data/2024Q4map.xlsx new file:   data/Q12024_13012025 .xlsx deleted:    data/Q12024_13012025.xlsx renamed:    pages/2024_Annual_Report.py -> pages/Q1-4_2024_Annual_Report.py modified:   pages/Q2_2024_Report.py modified:   pages/Q3_2024_Report.py modified:   pages/Q4_2024_Report.py
</commit_message>
<xml_diff>
--- a/data/2024Q3map.xlsx
+++ b/data/2024Q3map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nina/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5F445FB-65B9-484F-89FF-A81473F7E58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15031771-649A-3B4C-BAF2-D51F837EC5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24680" yWindow="1180" windowWidth="28040" windowHeight="17440" xr2:uid="{1725AB4C-30FF-F144-874F-AE8DBB3F0BFD}"/>
+    <workbookView xWindow="23160" yWindow="1180" windowWidth="28040" windowHeight="17440" xr2:uid="{1725AB4C-30FF-F144-874F-AE8DBB3F0BFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,15 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
-    <t>Institution</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longtitude</t>
-  </si>
-  <si>
     <t xml:space="preserve"> University of Cologne</t>
   </si>
   <si>
@@ -93,19 +84,34 @@
   </si>
   <si>
     <t>Open University of Catalunya</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,8 +134,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,7 +474,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,19 +483,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>60.385399999999997</v>
@@ -499,7 +506,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>50.933300000000003</v>
@@ -510,7 +517,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>43.657200000000003</v>
@@ -521,7 +528,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>51.34</v>
@@ -532,7 +539,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>69.649600000000007</v>
@@ -543,7 +550,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>44.058199999999999</v>
@@ -554,7 +561,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>45.813099999999999</v>
@@ -565,7 +572,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>45.814999999999998</v>
@@ -576,7 +583,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>64.135499999999993</v>
@@ -587,7 +594,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>-26.191099999999999</v>
@@ -598,7 +605,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>-26.146000000000001</v>
@@ -609,7 +616,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>61.499000000000002</v>
@@ -620,7 +627,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>50.819299999999998</v>
@@ -631,7 +638,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>51.2194</v>
@@ -642,7 +649,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>50.261000000000003</v>
@@ -653,7 +660,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>41.393000000000001</v>

</xml_diff>